<commit_message>
Fixed some typos in the 384 plate test file.
</commit_message>
<xml_diff>
--- a/tests/testthat/input_files/test384.xlsx
+++ b/tests/testthat/input_files/test384.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gage1\Documents\Work\RTQ_analysis\tests\testthat\input files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rowde002\Documents\quicR\tests\testthat\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A400B51A-870D-417B-982C-8F5EDE8C7340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F7B6DD-AE23-41BB-B182-CB8353CA946A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microplate Cycle 1 (0 h)" sheetId="2" r:id="rId1"/>
@@ -21,12 +21,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="430">
   <si>
     <t>User: USER</t>
   </si>
@@ -1544,7 +1547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1600,9 +1603,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1887,7 +1887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AA88"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
@@ -6260,8 +6260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:JF80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10302,7 +10302,9 @@
       </c>
     </row>
     <row r="16" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B16" s="1">
         <v>0</v>
       </c>
@@ -11100,7 +11102,9 @@
       </c>
     </row>
     <row r="17" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B17" s="1">
         <v>0.75</v>
       </c>
@@ -11898,7 +11902,9 @@
       </c>
     </row>
     <row r="18" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B18" s="1">
         <v>1.5</v>
       </c>
@@ -12696,7 +12702,9 @@
       </c>
     </row>
     <row r="19" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B19" s="1">
         <v>2.25</v>
       </c>
@@ -13494,7 +13502,9 @@
       </c>
     </row>
     <row r="20" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -14292,7 +14302,9 @@
       </c>
     </row>
     <row r="21" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="A21" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B21" s="1">
         <v>3.75</v>
       </c>
@@ -15090,7 +15102,9 @@
       </c>
     </row>
     <row r="22" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B22" s="1">
         <v>4.5</v>
       </c>
@@ -15888,7 +15902,9 @@
       </c>
     </row>
     <row r="23" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B23" s="1">
         <v>5.25</v>
       </c>
@@ -16686,7 +16702,9 @@
       </c>
     </row>
     <row r="24" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B24" s="1">
         <v>6</v>
       </c>
@@ -17484,7 +17502,9 @@
       </c>
     </row>
     <row r="25" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
+      <c r="A25" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B25" s="1">
         <v>6.75</v>
       </c>
@@ -18282,7 +18302,9 @@
       </c>
     </row>
     <row r="26" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+      <c r="A26" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B26" s="1">
         <v>7.5</v>
       </c>
@@ -19080,7 +19102,9 @@
       </c>
     </row>
     <row r="27" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
+      <c r="A27" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B27" s="1">
         <v>8.25</v>
       </c>
@@ -19878,7 +19902,9 @@
       </c>
     </row>
     <row r="28" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+      <c r="A28" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B28" s="1">
         <v>9</v>
       </c>
@@ -20676,7 +20702,9 @@
       </c>
     </row>
     <row r="29" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+      <c r="A29" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B29" s="1">
         <v>9.75</v>
       </c>
@@ -21474,7 +21502,9 @@
       </c>
     </row>
     <row r="30" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
+      <c r="A30" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B30" s="1">
         <v>10.5</v>
       </c>
@@ -22272,7 +22302,9 @@
       </c>
     </row>
     <row r="31" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+      <c r="A31" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B31" s="1">
         <v>11.25</v>
       </c>
@@ -23070,7 +23102,9 @@
       </c>
     </row>
     <row r="32" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
+      <c r="A32" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B32" s="1">
         <v>12</v>
       </c>
@@ -23868,7 +23902,9 @@
       </c>
     </row>
     <row r="33" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
+      <c r="A33" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B33" s="1">
         <v>12.75</v>
       </c>
@@ -24666,7 +24702,9 @@
       </c>
     </row>
     <row r="34" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
+      <c r="A34" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B34" s="1">
         <v>13.5</v>
       </c>
@@ -25464,7 +25502,9 @@
       </c>
     </row>
     <row r="35" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
+      <c r="A35" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B35" s="1">
         <v>14.25</v>
       </c>
@@ -26262,7 +26302,9 @@
       </c>
     </row>
     <row r="36" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+      <c r="A36" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B36" s="1">
         <v>15</v>
       </c>
@@ -27060,7 +27102,9 @@
       </c>
     </row>
     <row r="37" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
+      <c r="A37" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B37" s="1">
         <v>15.75</v>
       </c>
@@ -27858,7 +27902,9 @@
       </c>
     </row>
     <row r="38" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
+      <c r="A38" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B38" s="1">
         <v>16.5</v>
       </c>
@@ -28656,7 +28702,9 @@
       </c>
     </row>
     <row r="39" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
+      <c r="A39" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B39" s="1">
         <v>17.25</v>
       </c>
@@ -29454,7 +29502,9 @@
       </c>
     </row>
     <row r="40" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
+      <c r="A40" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B40" s="1">
         <v>18</v>
       </c>
@@ -30252,7 +30302,9 @@
       </c>
     </row>
     <row r="41" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+      <c r="A41" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B41" s="1">
         <v>18.75</v>
       </c>
@@ -31050,7 +31102,9 @@
       </c>
     </row>
     <row r="42" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A42" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B42" s="1">
         <v>19.5</v>
       </c>
@@ -31848,7 +31902,9 @@
       </c>
     </row>
     <row r="43" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
+      <c r="A43" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B43" s="1">
         <v>20.25</v>
       </c>
@@ -32646,7 +32702,9 @@
       </c>
     </row>
     <row r="44" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
+      <c r="A44" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B44" s="1">
         <v>21</v>
       </c>
@@ -33444,7 +33502,9 @@
       </c>
     </row>
     <row r="45" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+      <c r="A45" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B45" s="1">
         <v>21.75</v>
       </c>
@@ -34242,7 +34302,9 @@
       </c>
     </row>
     <row r="46" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
+      <c r="A46" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B46" s="1">
         <v>22.5</v>
       </c>
@@ -35040,7 +35102,9 @@
       </c>
     </row>
     <row r="47" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
+      <c r="A47" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B47" s="1">
         <v>23.25</v>
       </c>
@@ -35838,7 +35902,9 @@
       </c>
     </row>
     <row r="48" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
+      <c r="A48" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B48" s="1">
         <v>24</v>
       </c>
@@ -36636,7 +36702,9 @@
       </c>
     </row>
     <row r="49" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
+      <c r="A49" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B49" s="1">
         <v>24.75</v>
       </c>
@@ -37434,7 +37502,9 @@
       </c>
     </row>
     <row r="50" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
+      <c r="A50" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B50" s="1">
         <v>25.5</v>
       </c>
@@ -38232,7 +38302,9 @@
       </c>
     </row>
     <row r="51" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
+      <c r="A51" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B51" s="1">
         <v>26.25</v>
       </c>
@@ -39030,7 +39102,9 @@
       </c>
     </row>
     <row r="52" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
+      <c r="A52" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B52" s="1">
         <v>27</v>
       </c>
@@ -39828,7 +39902,9 @@
       </c>
     </row>
     <row r="53" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
+      <c r="A53" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B53" s="1">
         <v>27.75</v>
       </c>
@@ -40626,7 +40702,9 @@
       </c>
     </row>
     <row r="54" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
+      <c r="A54" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B54" s="1">
         <v>28.5</v>
       </c>
@@ -41424,7 +41502,9 @@
       </c>
     </row>
     <row r="55" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
+      <c r="A55" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B55" s="1">
         <v>29.25</v>
       </c>
@@ -42222,7 +42302,9 @@
       </c>
     </row>
     <row r="56" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
+      <c r="A56" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B56" s="1">
         <v>30</v>
       </c>
@@ -43020,7 +43102,9 @@
       </c>
     </row>
     <row r="57" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
+      <c r="A57" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B57" s="1">
         <v>30.75</v>
       </c>
@@ -43818,7 +43902,9 @@
       </c>
     </row>
     <row r="58" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
+      <c r="A58" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B58" s="1">
         <v>31.5</v>
       </c>
@@ -44616,7 +44702,9 @@
       </c>
     </row>
     <row r="59" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
+      <c r="A59" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B59" s="1">
         <v>32.25</v>
       </c>
@@ -45414,7 +45502,9 @@
       </c>
     </row>
     <row r="60" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
+      <c r="A60" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B60" s="1">
         <v>33</v>
       </c>
@@ -46212,7 +46302,9 @@
       </c>
     </row>
     <row r="61" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
+      <c r="A61" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B61" s="1">
         <v>33.75</v>
       </c>
@@ -47010,7 +47102,9 @@
       </c>
     </row>
     <row r="62" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
+      <c r="A62" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B62" s="1">
         <v>34.5</v>
       </c>
@@ -47808,7 +47902,9 @@
       </c>
     </row>
     <row r="63" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
+      <c r="A63" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B63" s="1">
         <v>35.25</v>
       </c>
@@ -48606,7 +48702,9 @@
       </c>
     </row>
     <row r="64" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
+      <c r="A64" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B64" s="1">
         <v>36</v>
       </c>
@@ -49404,7 +49502,9 @@
       </c>
     </row>
     <row r="65" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
+      <c r="A65" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B65" s="1">
         <v>36.75</v>
       </c>
@@ -50202,7 +50302,9 @@
       </c>
     </row>
     <row r="66" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
+      <c r="A66" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B66" s="1">
         <v>37.5</v>
       </c>
@@ -51000,7 +51102,9 @@
       </c>
     </row>
     <row r="67" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
+      <c r="A67" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B67" s="1">
         <v>38.25</v>
       </c>
@@ -51798,7 +51902,9 @@
       </c>
     </row>
     <row r="68" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A68" s="23"/>
+      <c r="A68" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B68" s="1">
         <v>39</v>
       </c>
@@ -52596,7 +52702,9 @@
       </c>
     </row>
     <row r="69" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A69" s="23"/>
+      <c r="A69" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B69" s="1">
         <v>39.75</v>
       </c>
@@ -53394,7 +53502,9 @@
       </c>
     </row>
     <row r="70" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
+      <c r="A70" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B70" s="1">
         <v>40.5</v>
       </c>
@@ -54192,7 +54302,9 @@
       </c>
     </row>
     <row r="71" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
+      <c r="A71" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B71" s="1">
         <v>41.25</v>
       </c>
@@ -54990,7 +55102,9 @@
       </c>
     </row>
     <row r="72" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
+      <c r="A72" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B72" s="1">
         <v>42</v>
       </c>
@@ -55788,7 +55902,9 @@
       </c>
     </row>
     <row r="73" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
+      <c r="A73" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B73" s="1">
         <v>42.75</v>
       </c>
@@ -56586,7 +56702,9 @@
       </c>
     </row>
     <row r="74" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
+      <c r="A74" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B74" s="1">
         <v>43.5</v>
       </c>
@@ -57384,7 +57502,9 @@
       </c>
     </row>
     <row r="75" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
+      <c r="A75" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B75" s="1">
         <v>44.25</v>
       </c>
@@ -58182,7 +58302,9 @@
       </c>
     </row>
     <row r="76" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
+      <c r="A76" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B76" s="1">
         <v>45</v>
       </c>
@@ -58980,7 +59102,9 @@
       </c>
     </row>
     <row r="77" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A77" s="23"/>
+      <c r="A77" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B77" s="1">
         <v>45.75</v>
       </c>
@@ -59778,7 +59902,9 @@
       </c>
     </row>
     <row r="78" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
+      <c r="A78" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B78" s="1">
         <v>46.5</v>
       </c>
@@ -60576,7 +60702,9 @@
       </c>
     </row>
     <row r="79" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A79" s="23"/>
+      <c r="A79" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B79" s="1">
         <v>47.25</v>
       </c>
@@ -61374,7 +61502,9 @@
       </c>
     </row>
     <row r="80" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A80" s="23"/>
+      <c r="A80" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B80" s="1">
         <v>48</v>
       </c>

</xml_diff>